<commit_message>
feat: add account name to db
</commit_message>
<xml_diff>
--- a/processed_file.xlsx
+++ b/processed_file.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I375"/>
+  <dimension ref="A1:J375"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -482,6 +487,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -511,6 +521,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -542,6 +557,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -573,6 +593,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -604,6 +629,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -635,6 +665,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -666,6 +701,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -697,6 +737,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -728,6 +773,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -759,6 +809,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -790,6 +845,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -821,6 +881,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -852,6 +917,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -883,6 +953,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -914,6 +989,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -945,6 +1025,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -976,6 +1061,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1007,6 +1097,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1038,6 +1133,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1069,6 +1169,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1100,6 +1205,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1131,6 +1241,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1162,6 +1277,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1193,6 +1313,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1224,6 +1349,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1255,6 +1385,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1286,6 +1421,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1317,6 +1457,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1348,6 +1493,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1379,6 +1529,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1410,6 +1565,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1441,6 +1601,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1472,6 +1637,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1503,6 +1673,11 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1534,6 +1709,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1565,6 +1745,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1596,6 +1781,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1627,6 +1817,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1658,6 +1853,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1689,6 +1889,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1720,6 +1925,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1751,6 +1961,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1782,6 +1997,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1813,6 +2033,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1844,6 +2069,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1875,6 +2105,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1906,6 +2141,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1937,6 +2177,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1968,6 +2213,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1999,6 +2249,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2030,6 +2285,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2061,6 +2321,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2092,6 +2357,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2123,6 +2393,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2154,6 +2429,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2185,6 +2465,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2216,6 +2501,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2245,6 +2535,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2274,6 +2569,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2303,6 +2603,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2332,6 +2637,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2363,6 +2673,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2394,6 +2709,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2425,6 +2745,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2456,6 +2781,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2487,6 +2817,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2518,6 +2853,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2549,6 +2889,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2580,6 +2925,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2611,6 +2961,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2642,6 +2997,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2673,6 +3033,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2704,6 +3069,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2735,6 +3105,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2766,6 +3141,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2797,6 +3177,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2828,6 +3213,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2859,6 +3249,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2890,6 +3285,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2921,6 +3321,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2952,6 +3357,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2983,6 +3393,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -3014,6 +3429,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -3045,6 +3465,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -3076,6 +3501,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -3107,6 +3537,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -3138,6 +3573,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -3169,6 +3609,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -3200,6 +3645,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -3231,6 +3681,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -3262,6 +3717,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -3293,6 +3753,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -3324,6 +3789,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -3355,6 +3825,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -3386,6 +3861,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -3417,6 +3897,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -3448,6 +3933,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -3479,6 +3969,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -3510,6 +4005,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -3541,6 +4041,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -3572,6 +4077,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3603,6 +4113,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -3634,6 +4149,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -3665,6 +4185,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -3696,6 +4221,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -3727,6 +4257,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -3758,6 +4293,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -3789,6 +4329,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -3820,6 +4365,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3851,6 +4401,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -3882,6 +4437,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -3913,6 +4473,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -3944,6 +4509,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -3975,6 +4545,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -4006,6 +4581,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -4037,6 +4617,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -4068,6 +4653,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -4099,6 +4689,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -4130,6 +4725,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -4161,6 +4761,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -4192,6 +4797,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -4223,6 +4833,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -4254,6 +4869,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -4285,6 +4905,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -4316,6 +4941,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -4347,6 +4977,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -4378,6 +5013,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -4409,6 +5049,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -4440,6 +5085,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -4471,6 +5121,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -4502,6 +5157,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -4533,6 +5193,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -4564,6 +5229,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -4595,6 +5265,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -4626,6 +5301,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -4657,6 +5337,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -4688,6 +5373,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -4719,6 +5409,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -4750,6 +5445,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -4781,6 +5481,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -4812,6 +5517,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -4843,6 +5553,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -4874,6 +5589,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -4905,6 +5625,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -4936,6 +5661,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -4967,6 +5697,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -4998,6 +5733,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -5029,6 +5769,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -5060,6 +5805,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -5091,6 +5841,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -5122,6 +5877,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -5153,6 +5913,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -5184,6 +5949,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -5215,6 +5985,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -5246,6 +6021,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -5275,6 +6055,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -5304,6 +6089,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -5335,6 +6125,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -5366,6 +6161,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -5397,6 +6197,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -5428,6 +6233,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -5459,6 +6269,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -5490,6 +6305,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -5521,6 +6341,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -5552,6 +6377,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -5583,6 +6413,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -5614,6 +6449,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -5645,6 +6485,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -5676,6 +6521,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -5707,6 +6557,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -5738,6 +6593,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -5769,6 +6629,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -5800,6 +6665,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -5831,6 +6701,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -5862,6 +6737,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -5893,6 +6773,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -5924,6 +6809,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -5955,6 +6845,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -5986,6 +6881,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -6017,6 +6917,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -6048,6 +6953,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -6079,6 +6989,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -6110,6 +7025,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -6141,6 +7061,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -6172,6 +7097,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -6203,6 +7133,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -6234,6 +7169,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -6265,6 +7205,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -6296,6 +7241,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -6327,6 +7277,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -6358,6 +7313,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -6389,6 +7349,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -6420,6 +7385,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -6451,6 +7421,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -6482,6 +7457,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -6513,6 +7493,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -6544,6 +7529,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -6573,6 +7563,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -6602,6 +7597,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -6633,6 +7633,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -6664,6 +7669,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -6695,6 +7705,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -6726,6 +7741,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -6757,6 +7777,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -6788,6 +7813,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -6819,6 +7849,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -6850,6 +7885,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -6881,6 +7921,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -6912,6 +7957,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -6943,6 +7993,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J211" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -6974,6 +8029,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J212" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -7005,6 +8065,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -7036,6 +8101,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -7067,6 +8137,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -7096,6 +8171,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J216" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -7127,6 +8207,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J217" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -7158,6 +8243,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J218" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -7189,6 +8279,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J219" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -7220,6 +8315,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J220" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -7251,6 +8351,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J221" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -7282,6 +8387,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J222" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -7313,6 +8423,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J223" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -7344,6 +8459,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J224" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -7375,6 +8495,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J225" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -7406,6 +8531,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J226" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -7437,6 +8567,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J227" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -7468,6 +8603,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J228" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -7499,6 +8639,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J229" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -7530,6 +8675,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J230" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -7561,6 +8711,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J231" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -7592,6 +8747,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J232" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -7623,6 +8783,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J233" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -7654,6 +8819,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J234" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -7685,6 +8855,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J235" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -7716,6 +8891,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J236" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -7747,6 +8927,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J237" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -7778,6 +8963,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J238" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -7809,6 +8999,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J239" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -7840,6 +9035,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J240" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -7871,6 +9071,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J241" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -7902,6 +9107,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J242" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -7933,6 +9143,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J243" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -7964,6 +9179,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J244" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -7995,6 +9215,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J245" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -8026,6 +9251,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J246" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -8057,6 +9287,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J247" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -8086,6 +9321,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J248" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -8115,6 +9355,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J249" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -8144,6 +9389,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J250" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -8173,6 +9423,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J251" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -8202,6 +9457,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J252" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -8231,6 +9491,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J253" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -8260,6 +9525,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J254" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -8289,6 +9559,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J255" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -8318,6 +9593,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J256" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -8347,6 +9627,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J257" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -8376,6 +9661,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J258" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -8405,6 +9695,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J259" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -8434,6 +9729,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J260" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -8463,6 +9763,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J261" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -8492,6 +9797,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J262" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -8521,6 +9831,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J263" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -8550,6 +9865,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J264" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -8579,6 +9899,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J265" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -8608,6 +9933,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J266" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -8637,6 +9967,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J267" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -8666,6 +10001,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J268" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -8695,6 +10035,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J269" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -8724,6 +10069,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J270" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -8753,6 +10103,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J271" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -8782,6 +10137,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J272" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -8811,6 +10171,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J273" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -8840,6 +10205,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J274" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -8869,6 +10239,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J275" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -8898,6 +10273,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J276" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -8927,6 +10307,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J277" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -8956,6 +10341,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J278" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -8985,6 +10375,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J279" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -9014,6 +10409,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J280" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -9043,6 +10443,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J281" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -9072,6 +10477,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J282" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -9101,6 +10511,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J283" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -9130,6 +10545,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J284" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -9159,6 +10579,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J285" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -9188,6 +10613,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J286" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -9217,6 +10647,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J287" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -9246,6 +10681,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J288" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -9275,6 +10715,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J289" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -9304,6 +10749,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J290" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -9333,6 +10783,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J291" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -9362,6 +10817,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J292" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -9391,6 +10851,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J293" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -9420,6 +10885,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J294" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -9449,6 +10919,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J295" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -9478,6 +10953,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J296" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -9507,6 +10987,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J297" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -9536,6 +11021,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J298" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -9565,6 +11055,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J299" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -9594,6 +11089,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J300" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -9623,6 +11123,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J301" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -9652,6 +11157,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J302" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -9681,6 +11191,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J303" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -9710,6 +11225,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J304" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
@@ -9739,6 +11259,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J305" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -9768,6 +11293,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J306" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
@@ -9797,6 +11327,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J307" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -9826,6 +11361,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J308" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -9855,6 +11395,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J309" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -9884,6 +11429,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J310" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -9913,6 +11463,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J311" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
@@ -9942,6 +11497,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J312" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
@@ -9971,6 +11531,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J313" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -10000,6 +11565,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J314" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
@@ -10029,6 +11599,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J315" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
@@ -10058,6 +11633,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J316" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
@@ -10087,6 +11667,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J317" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -10116,6 +11701,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J318" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -10145,6 +11735,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J319" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -10174,6 +11769,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J320" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -10203,6 +11803,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J321" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
@@ -10232,6 +11837,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J322" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
@@ -10261,6 +11871,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J323" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
@@ -10290,6 +11905,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J324" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
@@ -10319,6 +11939,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J325" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
@@ -10348,6 +11973,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J326" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
@@ -10377,6 +12007,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J327" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
@@ -10406,6 +12041,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J328" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -10435,6 +12075,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J329" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
@@ -10464,6 +12109,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J330" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -10493,6 +12143,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J331" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
@@ -10522,6 +12177,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J332" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
@@ -10551,6 +12211,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J333" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -10580,6 +12245,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J334" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
@@ -10609,6 +12279,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J335" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -10638,6 +12313,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J336" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -10667,6 +12347,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J337" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -10696,6 +12381,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J338" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
@@ -10725,6 +12415,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J339" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -10754,6 +12449,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J340" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
@@ -10783,6 +12483,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J341" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -10812,6 +12517,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J342" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
@@ -10841,6 +12551,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J343" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
@@ -10870,6 +12585,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J344" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
@@ -10899,6 +12619,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J345" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
@@ -10928,6 +12653,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J346" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
@@ -10957,6 +12687,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J347" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
@@ -10986,6 +12721,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J348" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
@@ -11015,6 +12755,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J349" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
@@ -11044,6 +12789,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J350" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
@@ -11073,6 +12823,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J351" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
@@ -11102,6 +12857,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J352" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
@@ -11131,6 +12891,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J353" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
@@ -11160,6 +12925,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J354" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
@@ -11189,6 +12959,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J355" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
@@ -11218,6 +12993,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J356" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
@@ -11247,6 +13027,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J357" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
@@ -11276,6 +13061,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J358" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
@@ -11305,6 +13095,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J359" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
@@ -11334,6 +13129,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J360" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
@@ -11363,6 +13163,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J361" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
@@ -11392,6 +13197,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J362" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
@@ -11421,6 +13231,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J363" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
@@ -11450,6 +13265,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J364" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
@@ -11479,6 +13299,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J365" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
@@ -11508,6 +13333,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J366" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
@@ -11537,6 +13367,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J367" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
@@ -11566,6 +13401,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J368" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
@@ -11595,6 +13435,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J369" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
@@ -11624,6 +13469,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J370" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
@@ -11653,6 +13503,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J371" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
@@ -11682,6 +13537,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J372" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
@@ -11711,6 +13571,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J373" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
@@ -11740,6 +13605,11 @@
           <t>C</t>
         </is>
       </c>
+      <c r="J374" t="inlineStr">
+        <is>
+          <t>30991</t>
+        </is>
+      </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
@@ -11767,6 +13637,11 @@
       <c r="I375" t="inlineStr">
         <is>
           <t>C</t>
+        </is>
+      </c>
+      <c r="J375" t="inlineStr">
+        <is>
+          <t>30991</t>
         </is>
       </c>
     </row>

</xml_diff>